<commit_message>
Modificacion Page y Steps
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Data.xlsx
+++ b/src/main/resources/Data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Documents\AUTOMATIZACION_BOCC\Haced\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7962D443-D97E-47B1-AF67-1E417BF25706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D78922-93AD-48D1-BCDB-78F4173258AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <t>Oliveros</t>
   </si>
   <si>
-    <t>alejoA-1998@yopmail.com</t>
+    <t>alejo1323-1998@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Modificacion Page y Steps -refactorizacion
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Data.xlsx
+++ b/src/main/resources/Data/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Documents\AUTOMATIZACION_BOCC\Haced\src\main\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Documents\AUTOMATIZACION_BOCC\Haceb\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D78922-93AD-48D1-BCDB-78F4173258AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8F77D8-12A7-465B-9F3D-27B4460E5EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,14 +85,14 @@
     <t>Oliveros</t>
   </si>
   <si>
-    <t>alejo1323-1998@yopmail.com</t>
+    <t>alejo1235@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +122,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,11 +151,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -425,7 +433,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -517,6 +525,9 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8" spans="1:12">
+      <c r="D8" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Modificacion de Steps DESCRIPCIONES + Abrir con CHROME
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/Data.xlsx
+++ b/src/main/resources/Data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Documents\AUTOMATIZACION_BOCC\Haceb\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8F77D8-12A7-465B-9F3D-27B4460E5EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3C3FB6-59CE-4A22-A8D1-D743146212E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
     <t>Oliveros</t>
   </si>
   <si>
-    <t>alejo1235@yopmail.com</t>
+    <t>alejo1335@yopmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>